<commit_message>
renumerar tablas capítulo 2
</commit_message>
<xml_diff>
--- a/Documento/tablas/tablas_tfm.xlsx
+++ b/Documento/tablas/tablas_tfm.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dredondo\Dropbox\Transporte_interno\Máster\Ciencia de Datos\TFM\Documento\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DC83B0-794D-4DD4-84A5-08130D2DD55C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C20BD61-4A7F-4845-A943-148011D41348}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1320" windowWidth="21340" windowHeight="17920" tabRatio="752" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="1320" windowWidth="21340" windowHeight="17920" tabRatio="752" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="10" r:id="rId1"/>
     <sheet name="Tabla 1 - Poblaciones estándar" sheetId="19" r:id="rId2"/>
-    <sheet name="Tabla X - Incidencia total EPNM" sheetId="20" r:id="rId3"/>
-    <sheet name="Tabla X - Incidencia hígado" sheetId="21" r:id="rId4"/>
-    <sheet name="Tabla X - Incidencia CR" sheetId="22" r:id="rId5"/>
-    <sheet name="Tabla X - Mortalidad total EPNM" sheetId="23" r:id="rId6"/>
-    <sheet name="Tabla X - Mortalidad hígado" sheetId="24" r:id="rId7"/>
-    <sheet name="Tabla X - Mortalidad CR" sheetId="25" r:id="rId8"/>
+    <sheet name="Tabla 2 - Incidencia total EPNM" sheetId="20" r:id="rId3"/>
+    <sheet name="Tabla 3 - Incidencia hígado" sheetId="21" r:id="rId4"/>
+    <sheet name="Tabla 4 - Incidencia CR" sheetId="22" r:id="rId5"/>
+    <sheet name="Tabla 5 - Mortalidad total EPNM" sheetId="23" r:id="rId6"/>
+    <sheet name="Tabla 6 - Mortalidad hígado" sheetId="24" r:id="rId7"/>
+    <sheet name="Tabla 7 - Mortalidad CR" sheetId="25" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1782,7 +1782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9436DE70-BD75-40BC-B5AC-9E5F6E635EB5}">
   <dimension ref="A4:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -4157,7 +4157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47DE4818-1CCF-446E-BC99-0CA1EECC75AD}">
   <dimension ref="A4:K29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G5" sqref="G5:I5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
actualizar capítulos 1 y 2
</commit_message>
<xml_diff>
--- a/Documento/tablas/tablas_tfm.xlsx
+++ b/Documento/tablas/tablas_tfm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dredondo\Dropbox\Transporte_interno\Máster\Ciencia de Datos\TFM\Documento\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845F9F43-A155-44CE-8B3B-BC5B58FAC1D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7C079F-0033-40FA-BD53-EFF2EDE084C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1320" windowWidth="21340" windowHeight="17920" tabRatio="752" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="1320" windowWidth="21340" windowHeight="17920" tabRatio="752" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="10" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="Tabla 5 - Mortalidad total EPNM" sheetId="23" r:id="rId6"/>
     <sheet name="Tabla 6 - Mortalidad hígado" sheetId="24" r:id="rId7"/>
     <sheet name="Tabla 7 - Mortalidad CR" sheetId="25" r:id="rId8"/>
-    <sheet name="Tabla X - Prevalencia" sheetId="26" r:id="rId9"/>
+    <sheet name="Tabla 8 - Supervivencia" sheetId="27" r:id="rId9"/>
+    <sheet name="Tabla 9 - Prevalencia" sheetId="26" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="225">
   <si>
     <t>Grupo de edad</t>
   </si>
@@ -669,13 +670,55 @@
   </si>
   <si>
     <t>17.895.356</t>
+  </si>
+  <si>
+    <t>Población y año</t>
+  </si>
+  <si>
+    <t>\begin{tabular}[c]{@{}c@{}}Mundo\\(años)\end{tabular}</t>
+  </si>
+  <si>
+    <t>\cite{Allemani2018}</t>
+  </si>
+  <si>
+    <t>\cite{Guevara2019}</t>
+  </si>
+  <si>
+    <t>\cite{DeAngelis2014, ECIS}</t>
+  </si>
+  <si>
+    <t>Sup obs 1 año</t>
+  </si>
+  <si>
+    <t>Sup rel 1 año</t>
+  </si>
+  <si>
+    <t>existe</t>
+  </si>
+  <si>
+    <t>\begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular}</t>
+  </si>
+  <si>
+    <t>y citar el informe de Guevara2019 con datos para 2002-2013</t>
+  </si>
+  <si>
+    <t>cambiar la cita de Guevara2019</t>
+  </si>
+  <si>
+    <t>\begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular}</t>
+  </si>
+  <si>
+    <t>Sup obs 5 año</t>
+  </si>
+  <si>
+    <t>Sup rel 5 año</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -753,6 +796,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -768,7 +819,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -806,13 +857,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -897,6 +959,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1242,6 +1306,713 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B244C3-CB16-495F-980A-6CB4471F2FAB}">
+  <dimension ref="A3:K32"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.25" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" t="s">
+        <v>147</v>
+      </c>
+      <c r="K5" s="9" t="str">
+        <f xml:space="preserve"> C5 &amp; " &amp; " &amp; D5 &amp; " &amp; " &amp; E5  &amp; " &amp; " &amp; F5 &amp; " &amp; " &amp; G5 &amp; " &amp; " &amp; H5 &amp; " &amp; " &amp; I5 &amp; "\\" &amp; IF(B5="x","\hline","")</f>
+        <v>Localización &amp; Sexo &amp; Población &amp; N &amp; Tasa &amp; N &amp; Tasa\\\hline</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="G6" s="31">
+        <v>145.6</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="I6" s="31">
+        <v>464.7</v>
+      </c>
+      <c r="K6" s="9" t="str">
+        <f xml:space="preserve"> C6 &amp; " &amp; " &amp; D6 &amp; " &amp; " &amp; E6  &amp; " &amp; " &amp; F6 &amp; " &amp; " &amp; G6 &amp; " &amp; " &amp; H6 &amp; " &amp; " &amp; I6 &amp; "\\" &amp; IF(B6="x"," \hline","") &amp; IF(A6="x"," \cline{2-7}","")</f>
+        <v>\multirow{9}{*}{Total del cáncer EPNM} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 5.607.801 &amp; 145,6 &amp; 17.895.356 &amp; 464,7\\</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D7" s="12"/>
+      <c r="E7" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="31">
+        <v>418.4</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="I7" s="31">
+        <v>1414.7</v>
+      </c>
+      <c r="K7" s="9" t="str">
+        <f t="shared" ref="K7:K32" si="0" xml:space="preserve"> C7 &amp; " &amp; " &amp; D7 &amp; " &amp; " &amp; E7  &amp; " &amp; " &amp; F7 &amp; " &amp; " &amp; G7 &amp; " &amp; " &amp; H7 &amp; " &amp; " &amp; I7 &amp; "\\" &amp; IF(B7="x"," \hline","") &amp; IF(A7="x"," \cline{2-7}","")</f>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 1.504.232 &amp; 418,4 &amp; 5.086.515 &amp; 1414,7\\</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="I8" s="31">
+        <v>1566.3</v>
+      </c>
+      <c r="K8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 105.599 &amp; 464,0 &amp; 356.427 &amp; 1566,3\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="G9" s="31">
+        <v>150.4</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="I9" s="31">
+        <v>548.29999999999995</v>
+      </c>
+      <c r="K9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 5.688.175 &amp; 150,4 &amp; 20.738.064 &amp; 548,3\\</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E10" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" s="31">
+        <v>373.4</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="I10" s="31">
+        <v>1409.8</v>
+      </c>
+      <c r="K10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 1.434.849 &amp; 373,4 &amp; 5.417.680 &amp; 1409,8\\</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="I11" s="31">
+        <v>1363.5</v>
+      </c>
+      <c r="K11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 84.409 &amp; 357,0 &amp; 322.341 &amp; 1363,5\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="I12" s="31">
+        <v>506.1</v>
+      </c>
+      <c r="K12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 11.295.976 &amp; 148,0 &amp; 38.633.420 &amp; 506,1\\</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E13" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="G13" s="31">
+        <v>395.1</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="I13" s="31">
+        <v>1412.2</v>
+      </c>
+      <c r="K13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 2.939.081 &amp; 395,1 &amp; 10.504.195 &amp; 1412,2\\</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="G14" s="31">
+        <v>409.5</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="I14" s="31">
+        <v>1462.9</v>
+      </c>
+      <c r="K14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 190.008 &amp; 409,5 &amp; 678.768 &amp; 1462,9\\ \hline</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="G15" s="32">
+        <v>6.1</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="I15" s="32">
+        <v>12.2</v>
+      </c>
+      <c r="K15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>\multirow{9}{*}{Hígado} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 236.669 &amp; 6,1 &amp; 471.525 &amp; 12,2\\</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D16" s="12"/>
+      <c r="E16" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="G16" s="33">
+        <v>5.9</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="I16" s="32">
+        <v>11.1</v>
+      </c>
+      <c r="K16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 21.240 &amp; 5,9 &amp; 39.867 &amp; 11,1\\</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="G17" s="33">
+        <v>8.5</v>
+      </c>
+      <c r="H17" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="I17" s="33">
+        <v>15.9</v>
+      </c>
+      <c r="K17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 1.924 &amp; 8,5 &amp; 3.618 &amp; 15,9\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="G18" s="32">
+        <v>2.6</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="I18" s="32">
+        <v>5.4</v>
+      </c>
+      <c r="K18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 97.621 &amp; 2,6 &amp; 203.685 &amp; 5,4\\</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E19" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="G19" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="I19" s="32">
+        <v>4.8</v>
+      </c>
+      <c r="K19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 9.719 &amp; 2,5 &amp; 18.610 &amp; 4,8\\</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="33">
+        <v>580</v>
+      </c>
+      <c r="G20" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="H20" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="I20" s="33">
+        <v>4.7</v>
+      </c>
+      <c r="K20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 580 &amp; 2,5 &amp; 1.102 &amp; 4,7\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="G21" s="32">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="I21" s="32">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 334.290 &amp; 4,4 &amp; 675.210 &amp; 8,8\\</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E22" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="G22" s="33">
+        <v>4.2</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="I22" s="32">
+        <v>7.9</v>
+      </c>
+      <c r="K22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 30.959 &amp; 4,2 &amp; 58.477 &amp; 7,9\\</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="G23" s="33">
+        <v>5.4</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="I23" s="33">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 2.504 &amp; 5,4 &amp; 4.720 &amp; 10,2\\ \hline</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" s="32">
+        <v>19.5</v>
+      </c>
+      <c r="H24" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="I24" s="32">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="K24" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>\multirow{9}{*}{Colon-recto} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 749.774 &amp; 19,5 &amp; 2.595.326 &amp; 67,4\\</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D25" s="12"/>
+      <c r="E25" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="G25" s="33">
+        <v>59.3</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="I25" s="32">
+        <v>208.2</v>
+      </c>
+      <c r="K25" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 213.233 &amp; 59,3 &amp; 748.455 &amp; 208,2\\</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="G26" s="33">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="H26" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="I26" s="33">
+        <v>279.5</v>
+      </c>
+      <c r="K26" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 18.059 &amp; 79,4 &amp; 63.593 &amp; 279,5\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="K27" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 606.377 &amp; 16,0 &amp; 2.194.309 &amp; 58,0\\</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E28" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="G28" s="33">
+        <v>46.6</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="I28" s="32">
+        <v>170.6</v>
+      </c>
+      <c r="K28" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 178.969 &amp; 46,6 &amp; 655.422 &amp; 170,6\\</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="G29" s="33">
+        <v>48.5</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="I29" s="33">
+        <v>178.2</v>
+      </c>
+      <c r="K29" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 11.463 &amp; 48,5 &amp; 42.121 &amp; 178,2\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="G30" s="32">
+        <v>17.8</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="I30" s="32">
+        <v>62.8</v>
+      </c>
+      <c r="K30" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 1.356.151 &amp; 17,8 &amp; 4.789.635 &amp; 62,8\\</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E31" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="G31" s="33">
+        <v>52.7</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="I31" s="32">
+        <v>188.7</v>
+      </c>
+      <c r="K31" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 392.202 &amp; 52,7 &amp; 1.403.877 &amp; 188,7\\</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="G32" s="33">
+        <v>63.6</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="I32" s="33">
+        <v>227.8</v>
+      </c>
+      <c r="K32" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 29.522 &amp; 63,6 &amp; 105.714 &amp; 227,8\\ \hline</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2715EA62-B995-4B2C-B81F-34E9E60572DB}">
   <dimension ref="A1:H43"/>
@@ -4840,21 +5611,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B244C3-CB16-495F-980A-6CB4471F2FAB}">
-  <dimension ref="A3:K32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82833DD-B50C-4E21-A8FA-CE9B4A74514D}">
+  <dimension ref="A3:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>152</v>
       </c>
@@ -4862,19 +5634,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H4" t="s">
-        <v>149</v>
-      </c>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -4885,26 +5651,29 @@
         <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>211</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="G5" t="s">
-        <v>147</v>
+        <v>216</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>217</v>
       </c>
       <c r="I5" t="s">
-        <v>147</v>
-      </c>
-      <c r="K5" s="9" t="str">
-        <f xml:space="preserve"> C5 &amp; " &amp; " &amp; D5 &amp; " &amp; " &amp; E5  &amp; " &amp; " &amp; F5 &amp; " &amp; " &amp; G5 &amp; " &amp; " &amp; H5 &amp; " &amp; " &amp; I5 &amp; "\\" &amp; IF(B5="x","\hline","")</f>
-        <v>Localización &amp; Sexo &amp; Población &amp; N &amp; Tasa &amp; N &amp; Tasa\\\hline</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+      <c r="J5" t="s">
+        <v>224</v>
+      </c>
+      <c r="L5" s="9" t="str">
+        <f xml:space="preserve"> C5 &amp; " &amp; " &amp; D5 &amp; " &amp; " &amp; E5  &amp; " &amp; " &amp; G5 &amp; " &amp; " &amp; H5 &amp; " &amp; " &amp; I5 &amp; " &amp; " &amp; J5 &amp; "\\" &amp; IF(B5="x","\hline","")</f>
+        <v>Localización &amp; Sexo &amp; Población y año &amp; Sup obs 1 año &amp; Sup rel 1 año &amp; Sup obs 5 año &amp; Sup rel 5 año\\\hline</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>146</v>
       </c>
@@ -4912,632 +5681,361 @@
         <v>77</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="G6" s="31">
-        <v>145.6</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="I6" s="31">
-        <v>464.7</v>
-      </c>
-      <c r="K6" s="9" t="str">
-        <f xml:space="preserve"> C6 &amp; " &amp; " &amp; D6 &amp; " &amp; " &amp; E6  &amp; " &amp; " &amp; F6 &amp; " &amp; " &amp; G6 &amp; " &amp; " &amp; H6 &amp; " &amp; " &amp; I6 &amp; "\\" &amp; IF(B6="x"," \hline","") &amp; IF(A6="x"," \cline{2-7}","")</f>
-        <v>\multirow{9}{*}{Total del cáncer EPNM} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 5.607.801 &amp; 145,6 &amp; 17.895.356 &amp; 464,7\\</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="L6" s="9" t="str">
+        <f xml:space="preserve"> C6 &amp; " &amp; " &amp; D6 &amp; " &amp; " &amp; E6  &amp; " &amp; " &amp; G6 &amp; " &amp; " &amp; H6 &amp; " &amp; " &amp; I6 &amp; " &amp; " &amp; J6 &amp; "\\" &amp; IF(B6="x"," \hline","") &amp; IF(A6="x"," \cline{2-7}","")</f>
+        <v>\multirow{9}{*}{Total del cáncer EPNM} &amp; \multirow{3}{*}{Hombres} &amp; \begin{tabular}[c]{@{}c@{}}Mundo\\(años)\end{tabular} &amp;  &amp;  &amp;  &amp; existe\\</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="12"/>
       <c r="E7" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="G7" s="31">
-        <v>418.4</v>
+        <v>219</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>218</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>209</v>
-      </c>
-      <c r="I7" s="31">
-        <v>1414.7</v>
-      </c>
-      <c r="K7" s="9" t="str">
-        <f t="shared" ref="K7:K32" si="0" xml:space="preserve"> C7 &amp; " &amp; " &amp; D7 &amp; " &amp; " &amp; E7  &amp; " &amp; " &amp; F7 &amp; " &amp; " &amp; G7 &amp; " &amp; " &amp; H7 &amp; " &amp; " &amp; I7 &amp; "\\" &amp; IF(B7="x"," \hline","") &amp; IF(A7="x"," \cline{2-7}","")</f>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 1.504.232 &amp; 418,4 &amp; 5.086.515 &amp; 1414,7\\</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>218</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="L7" s="9" t="str">
+        <f t="shared" ref="L7:L23" si="0" xml:space="preserve"> C7 &amp; " &amp; " &amp; D7 &amp; " &amp; " &amp; E7  &amp; " &amp; " &amp; G7 &amp; " &amp; " &amp; H7 &amp; " &amp; " &amp; I7 &amp; " &amp; " &amp; J7 &amp; "\\" &amp; IF(B7="x"," \hline","") &amp; IF(A7="x"," \cline{2-7}","")</f>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp; existe &amp; existe &amp; existe &amp; existe\\</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>153</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="G8" s="31"/>
       <c r="H8" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="I8" s="31">
-        <v>1566.3</v>
-      </c>
-      <c r="K8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 105.599 &amp; 464,0 &amp; 356.427 &amp; 1566,3\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>218</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="L8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp; existe &amp; existe &amp; existe\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>78</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="G9" s="31">
-        <v>150.4</v>
-      </c>
-      <c r="H9" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="I9" s="31">
-        <v>548.29999999999995</v>
-      </c>
-      <c r="K9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 5.688.175 &amp; 150,4 &amp; 20.738.064 &amp; 548,3\\</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F9" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="L9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp;  &amp;  &amp;  &amp; \\</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E10" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="G10" s="31">
-        <v>373.4</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="I10" s="31">
-        <v>1409.8</v>
-      </c>
-      <c r="K10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 1.434.849 &amp; 373,4 &amp; 5.417.680 &amp; 1409,8\\</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>219</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="L10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="I11" s="31">
-        <v>1363.5</v>
-      </c>
-      <c r="K11" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 84.409 &amp; 357,0 &amp; 322.341 &amp; 1363,5\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="L11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>145</v>
+      </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="I12" s="31">
-        <v>506.1</v>
-      </c>
-      <c r="K12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 11.295.976 &amp; 148,0 &amp; 38.633.420 &amp; 506,1\\</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F12" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="L12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>\multirow{9}{*}{Hígado} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp;  &amp;  &amp;  &amp; \\</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D13" s="12"/>
       <c r="E13" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="G13" s="31">
-        <v>395.1</v>
-      </c>
-      <c r="H13" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="I13" s="31">
-        <v>1412.2</v>
-      </c>
-      <c r="K13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 2.939.081 &amp; 395,1 &amp; 10.504.195 &amp; 1412,2\\</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+        <v>219</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="L13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>23</v>
       </c>
+      <c r="D14" s="12"/>
       <c r="E14" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="G14" s="31">
-        <v>409.5</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="I14" s="31">
-        <v>1462.9</v>
-      </c>
-      <c r="K14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 190.008 &amp; 409,5 &amp; 678.768 &amp; 1462,9\\ \hline</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
-        <v>145</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="L14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="G15" s="32">
-        <v>6.1</v>
-      </c>
-      <c r="H15" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="I15" s="32">
-        <v>12.2</v>
-      </c>
-      <c r="K15" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>\multirow{9}{*}{Hígado} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 236.669 &amp; 6,1 &amp; 471.525 &amp; 12,2\\</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D16" s="12"/>
+      <c r="F15" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="L15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp;  &amp;  &amp;  &amp; \\</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E16" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="G16" s="33">
-        <v>5.9</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="I16" s="32">
-        <v>11.1</v>
-      </c>
-      <c r="K16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 21.240 &amp; 5,9 &amp; 39.867 &amp; 11,1\\</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+        <v>219</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="L16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="12"/>
       <c r="E17" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="G17" s="33">
-        <v>8.5</v>
-      </c>
-      <c r="H17" s="33" t="s">
-        <v>199</v>
-      </c>
-      <c r="I17" s="33">
-        <v>15.9</v>
-      </c>
-      <c r="K17" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 1.924 &amp; 8,5 &amp; 3.618 &amp; 15,9\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="L17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>150</v>
+      </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="G18" s="32">
-        <v>2.6</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="I18" s="32">
-        <v>5.4</v>
-      </c>
-      <c r="K18" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 97.621 &amp; 2,6 &amp; 203.685 &amp; 5,4\\</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F18" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="L18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>\multirow{9}{*}{Colon-recto} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp;  &amp;  &amp;  &amp; \\</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D19" s="12"/>
       <c r="E19" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="G19" s="33">
-        <v>2.5</v>
-      </c>
-      <c r="H19" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="I19" s="32">
-        <v>4.8</v>
-      </c>
-      <c r="K19" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 9.719 &amp; 2,5 &amp; 18.610 &amp; 4,8\\</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+        <v>219</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="L19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
+      <c r="D20" s="12"/>
       <c r="E20" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="33">
-        <v>580</v>
-      </c>
-      <c r="G20" s="33">
-        <v>2.5</v>
-      </c>
-      <c r="H20" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="I20" s="33">
-        <v>4.7</v>
-      </c>
-      <c r="K20" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 580 &amp; 2,5 &amp; 1.102 &amp; 4,7\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="L20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="G21" s="32">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H21" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="I21" s="32">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="K21" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 334.290 &amp; 4,4 &amp; 675.210 &amp; 8,8\\</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F21" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="L21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp;  &amp;  &amp;  &amp; \\</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E22" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="G22" s="33">
-        <v>4.2</v>
-      </c>
-      <c r="H22" s="32" t="s">
-        <v>194</v>
-      </c>
-      <c r="I22" s="32">
-        <v>7.9</v>
-      </c>
-      <c r="K22" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 30.959 &amp; 4,2 &amp; 58.477 &amp; 7,9\\</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
+        <v>219</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="L22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="G23" s="33">
-        <v>5.4</v>
-      </c>
-      <c r="H23" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="I23" s="33">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="K23" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 2.504 &amp; 5,4 &amp; 4.720 &amp; 10,2\\ \hline</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="G24" s="32">
-        <v>19.5</v>
-      </c>
-      <c r="H24" s="32" t="s">
-        <v>192</v>
-      </c>
-      <c r="I24" s="32">
-        <v>67.400000000000006</v>
-      </c>
-      <c r="K24" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>\multirow{9}{*}{Colon-recto} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 749.774 &amp; 19,5 &amp; 2.595.326 &amp; 67,4\\</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D25" s="12"/>
-      <c r="E25" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="G25" s="33">
-        <v>59.3</v>
-      </c>
-      <c r="H25" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="I25" s="32">
-        <v>208.2</v>
-      </c>
-      <c r="K25" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 213.233 &amp; 59,3 &amp; 748.455 &amp; 208,2\\</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="G26" s="33">
-        <v>79.400000000000006</v>
-      </c>
-      <c r="H26" s="33" t="s">
-        <v>190</v>
-      </c>
-      <c r="I26" s="33">
-        <v>279.5</v>
-      </c>
-      <c r="K26" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 18.059 &amp; 79,4 &amp; 63.593 &amp; 279,5\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D27" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="H27" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="I27" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="K27" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 606.377 &amp; 16,0 &amp; 2.194.309 &amp; 58,0\\</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E28" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="G28" s="33">
-        <v>46.6</v>
-      </c>
-      <c r="H28" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="I28" s="32">
-        <v>170.6</v>
-      </c>
-      <c r="K28" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 178.969 &amp; 46,6 &amp; 655.422 &amp; 170,6\\</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="G29" s="33">
-        <v>48.5</v>
-      </c>
-      <c r="H29" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="I29" s="33">
-        <v>178.2</v>
-      </c>
-      <c r="K29" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 11.463 &amp; 48,5 &amp; 42.121 &amp; 178,2\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="G30" s="32">
-        <v>17.8</v>
-      </c>
-      <c r="H30" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="I30" s="32">
-        <v>62.8</v>
-      </c>
-      <c r="K30" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 1.356.151 &amp; 17,8 &amp; 4.789.635 &amp; 62,8\\</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E31" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="G31" s="33">
-        <v>52.7</v>
-      </c>
-      <c r="H31" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="I31" s="32">
-        <v>188.7</v>
-      </c>
-      <c r="K31" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 392.202 &amp; 52,7 &amp; 1.403.877 &amp; 188,7\\</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="G32" s="33">
-        <v>63.6</v>
-      </c>
-      <c r="H32" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="I32" s="33">
-        <v>227.8</v>
-      </c>
-      <c r="K32" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 29.522 &amp; 63,6 &amp; 105.714 &amp; 227,8\\ \hline</v>
+        <v>222</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="L23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E27" s="35" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E28" s="34" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizar saltos de línea a Mac
</commit_message>
<xml_diff>
--- a/Documento/tablas/tablas_tfm.xlsx
+++ b/Documento/tablas/tablas_tfm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dredondo\Dropbox\Transporte_interno\Máster\Ciencia de Datos\TFM\Documento\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7C079F-0033-40FA-BD53-EFF2EDE084C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B80B5BB-25B9-4C11-BF07-3B04E096873F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1320" windowWidth="21340" windowHeight="17920" tabRatio="752" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="917" yWindow="1320" windowWidth="21343" windowHeight="17923" tabRatio="752" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="10" r:id="rId1"/>
@@ -21,8 +21,7 @@
     <sheet name="Tabla 5 - Mortalidad total EPNM" sheetId="23" r:id="rId6"/>
     <sheet name="Tabla 6 - Mortalidad hígado" sheetId="24" r:id="rId7"/>
     <sheet name="Tabla 7 - Mortalidad CR" sheetId="25" r:id="rId8"/>
-    <sheet name="Tabla 8 - Supervivencia" sheetId="27" r:id="rId9"/>
-    <sheet name="Tabla 9 - Prevalencia" sheetId="26" r:id="rId10"/>
+    <sheet name="Tabla 8 - Prevalencia" sheetId="26" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="211">
   <si>
     <t>Grupo de edad</t>
   </si>
@@ -670,55 +669,13 @@
   </si>
   <si>
     <t>17.895.356</t>
-  </si>
-  <si>
-    <t>Población y año</t>
-  </si>
-  <si>
-    <t>\begin{tabular}[c]{@{}c@{}}Mundo\\(años)\end{tabular}</t>
-  </si>
-  <si>
-    <t>\cite{Allemani2018}</t>
-  </si>
-  <si>
-    <t>\cite{Guevara2019}</t>
-  </si>
-  <si>
-    <t>\cite{DeAngelis2014, ECIS}</t>
-  </si>
-  <si>
-    <t>Sup obs 1 año</t>
-  </si>
-  <si>
-    <t>Sup rel 1 año</t>
-  </si>
-  <si>
-    <t>existe</t>
-  </si>
-  <si>
-    <t>\begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular}</t>
-  </si>
-  <si>
-    <t>y citar el informe de Guevara2019 con datos para 2002-2013</t>
-  </si>
-  <si>
-    <t>cambiar la cita de Guevara2019</t>
-  </si>
-  <si>
-    <t>\begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular}</t>
-  </si>
-  <si>
-    <t>Sup obs 5 año</t>
-  </si>
-  <si>
-    <t>Sup rel 5 año</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -796,14 +753,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -819,7 +768,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -857,24 +806,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -959,8 +897,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1256,14 +1192,14 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>25</v>
       </c>
@@ -1271,17 +1207,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
       <c r="E5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>29</v>
       </c>
@@ -1289,12 +1225,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>28</v>
       </c>
@@ -1303,713 +1239,6 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B244C3-CB16-495F-980A-6CB4471F2FAB}">
-  <dimension ref="A3:K32"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H4" t="s">
-        <v>149</v>
-      </c>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" t="s">
-        <v>147</v>
-      </c>
-      <c r="H5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" t="s">
-        <v>147</v>
-      </c>
-      <c r="K5" s="9" t="str">
-        <f xml:space="preserve"> C5 &amp; " &amp; " &amp; D5 &amp; " &amp; " &amp; E5  &amp; " &amp; " &amp; F5 &amp; " &amp; " &amp; G5 &amp; " &amp; " &amp; H5 &amp; " &amp; " &amp; I5 &amp; "\\" &amp; IF(B5="x","\hline","")</f>
-        <v>Localización &amp; Sexo &amp; Población &amp; N &amp; Tasa &amp; N &amp; Tasa\\\hline</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="G6" s="31">
-        <v>145.6</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="I6" s="31">
-        <v>464.7</v>
-      </c>
-      <c r="K6" s="9" t="str">
-        <f xml:space="preserve"> C6 &amp; " &amp; " &amp; D6 &amp; " &amp; " &amp; E6  &amp; " &amp; " &amp; F6 &amp; " &amp; " &amp; G6 &amp; " &amp; " &amp; H6 &amp; " &amp; " &amp; I6 &amp; "\\" &amp; IF(B6="x"," \hline","") &amp; IF(A6="x"," \cline{2-7}","")</f>
-        <v>\multirow{9}{*}{Total del cáncer EPNM} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 5.607.801 &amp; 145,6 &amp; 17.895.356 &amp; 464,7\\</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D7" s="12"/>
-      <c r="E7" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="G7" s="31">
-        <v>418.4</v>
-      </c>
-      <c r="H7" s="31" t="s">
-        <v>209</v>
-      </c>
-      <c r="I7" s="31">
-        <v>1414.7</v>
-      </c>
-      <c r="K7" s="9" t="str">
-        <f t="shared" ref="K7:K32" si="0" xml:space="preserve"> C7 &amp; " &amp; " &amp; D7 &amp; " &amp; " &amp; E7  &amp; " &amp; " &amp; F7 &amp; " &amp; " &amp; G7 &amp; " &amp; " &amp; H7 &amp; " &amp; " &amp; I7 &amp; "\\" &amp; IF(B7="x"," \hline","") &amp; IF(A7="x"," \cline{2-7}","")</f>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 1.504.232 &amp; 418,4 &amp; 5.086.515 &amp; 1414,7\\</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="I8" s="31">
-        <v>1566.3</v>
-      </c>
-      <c r="K8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 105.599 &amp; 464,0 &amp; 356.427 &amp; 1566,3\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="G9" s="31">
-        <v>150.4</v>
-      </c>
-      <c r="H9" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="I9" s="31">
-        <v>548.29999999999995</v>
-      </c>
-      <c r="K9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 5.688.175 &amp; 150,4 &amp; 20.738.064 &amp; 548,3\\</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E10" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="G10" s="31">
-        <v>373.4</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="I10" s="31">
-        <v>1409.8</v>
-      </c>
-      <c r="K10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 1.434.849 &amp; 373,4 &amp; 5.417.680 &amp; 1409,8\\</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="I11" s="31">
-        <v>1363.5</v>
-      </c>
-      <c r="K11" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 84.409 &amp; 357,0 &amp; 322.341 &amp; 1363,5\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="I12" s="31">
-        <v>506.1</v>
-      </c>
-      <c r="K12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 11.295.976 &amp; 148,0 &amp; 38.633.420 &amp; 506,1\\</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E13" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="G13" s="31">
-        <v>395.1</v>
-      </c>
-      <c r="H13" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="I13" s="31">
-        <v>1412.2</v>
-      </c>
-      <c r="K13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 2.939.081 &amp; 395,1 &amp; 10.504.195 &amp; 1412,2\\</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="G14" s="31">
-        <v>409.5</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="I14" s="31">
-        <v>1462.9</v>
-      </c>
-      <c r="K14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 190.008 &amp; 409,5 &amp; 678.768 &amp; 1462,9\\ \hline</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
-        <v>145</v>
-      </c>
-      <c r="D15" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="G15" s="32">
-        <v>6.1</v>
-      </c>
-      <c r="H15" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="I15" s="32">
-        <v>12.2</v>
-      </c>
-      <c r="K15" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>\multirow{9}{*}{Hígado} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 236.669 &amp; 6,1 &amp; 471.525 &amp; 12,2\\</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D16" s="12"/>
-      <c r="E16" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="G16" s="33">
-        <v>5.9</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="I16" s="32">
-        <v>11.1</v>
-      </c>
-      <c r="K16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 21.240 &amp; 5,9 &amp; 39.867 &amp; 11,1\\</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="G17" s="33">
-        <v>8.5</v>
-      </c>
-      <c r="H17" s="33" t="s">
-        <v>199</v>
-      </c>
-      <c r="I17" s="33">
-        <v>15.9</v>
-      </c>
-      <c r="K17" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 1.924 &amp; 8,5 &amp; 3.618 &amp; 15,9\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="G18" s="32">
-        <v>2.6</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="I18" s="32">
-        <v>5.4</v>
-      </c>
-      <c r="K18" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 97.621 &amp; 2,6 &amp; 203.685 &amp; 5,4\\</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E19" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="G19" s="33">
-        <v>2.5</v>
-      </c>
-      <c r="H19" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="I19" s="32">
-        <v>4.8</v>
-      </c>
-      <c r="K19" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 9.719 &amp; 2,5 &amp; 18.610 &amp; 4,8\\</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="33">
-        <v>580</v>
-      </c>
-      <c r="G20" s="33">
-        <v>2.5</v>
-      </c>
-      <c r="H20" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="I20" s="33">
-        <v>4.7</v>
-      </c>
-      <c r="K20" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 580 &amp; 2,5 &amp; 1.102 &amp; 4,7\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="G21" s="32">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H21" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="I21" s="32">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="K21" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 334.290 &amp; 4,4 &amp; 675.210 &amp; 8,8\\</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E22" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="G22" s="33">
-        <v>4.2</v>
-      </c>
-      <c r="H22" s="32" t="s">
-        <v>194</v>
-      </c>
-      <c r="I22" s="32">
-        <v>7.9</v>
-      </c>
-      <c r="K22" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 30.959 &amp; 4,2 &amp; 58.477 &amp; 7,9\\</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="G23" s="33">
-        <v>5.4</v>
-      </c>
-      <c r="H23" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="I23" s="33">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="K23" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 2.504 &amp; 5,4 &amp; 4.720 &amp; 10,2\\ \hline</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="G24" s="32">
-        <v>19.5</v>
-      </c>
-      <c r="H24" s="32" t="s">
-        <v>192</v>
-      </c>
-      <c r="I24" s="32">
-        <v>67.400000000000006</v>
-      </c>
-      <c r="K24" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>\multirow{9}{*}{Colon-recto} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 749.774 &amp; 19,5 &amp; 2.595.326 &amp; 67,4\\</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D25" s="12"/>
-      <c r="E25" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="G25" s="33">
-        <v>59.3</v>
-      </c>
-      <c r="H25" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="I25" s="32">
-        <v>208.2</v>
-      </c>
-      <c r="K25" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 213.233 &amp; 59,3 &amp; 748.455 &amp; 208,2\\</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="G26" s="33">
-        <v>79.400000000000006</v>
-      </c>
-      <c r="H26" s="33" t="s">
-        <v>190</v>
-      </c>
-      <c r="I26" s="33">
-        <v>279.5</v>
-      </c>
-      <c r="K26" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 18.059 &amp; 79,4 &amp; 63.593 &amp; 279,5\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D27" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="H27" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="I27" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="K27" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 606.377 &amp; 16,0 &amp; 2.194.309 &amp; 58,0\\</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E28" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="G28" s="33">
-        <v>46.6</v>
-      </c>
-      <c r="H28" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="I28" s="32">
-        <v>170.6</v>
-      </c>
-      <c r="K28" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 178.969 &amp; 46,6 &amp; 655.422 &amp; 170,6\\</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="G29" s="33">
-        <v>48.5</v>
-      </c>
-      <c r="H29" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="I29" s="33">
-        <v>178.2</v>
-      </c>
-      <c r="K29" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 11.463 &amp; 48,5 &amp; 42.121 &amp; 178,2\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="G30" s="32">
-        <v>17.8</v>
-      </c>
-      <c r="H30" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="I30" s="32">
-        <v>62.8</v>
-      </c>
-      <c r="K30" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 1.356.151 &amp; 17,8 &amp; 4.789.635 &amp; 62,8\\</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E31" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="G31" s="33">
-        <v>52.7</v>
-      </c>
-      <c r="H31" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="I31" s="32">
-        <v>188.7</v>
-      </c>
-      <c r="K31" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 392.202 &amp; 52,7 &amp; 1.403.877 &amp; 188,7\\</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="G32" s="33">
-        <v>63.6</v>
-      </c>
-      <c r="H32" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="I32" s="33">
-        <v>227.8</v>
-      </c>
-      <c r="K32" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; España &amp; 29.522 &amp; 63,6 &amp; 105.714 &amp; 227,8\\ \hline</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2021,26 +1250,26 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.640625" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="10.6640625" style="1"/>
+    <col min="1" max="2" width="10.640625" style="1"/>
     <col min="3" max="6" width="13.5" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="1"/>
-    <col min="8" max="8" width="36.08203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.6640625" style="1"/>
+    <col min="7" max="7" width="10.640625" style="1"/>
+    <col min="8" max="8" width="36.0703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="72.900000000000006" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2061,7 +1290,7 @@
         <v>Grupo de edad  &amp;  \begin{tabular}[c]{@{}r@{}}Población estándar\\ mundial\end{tabular}  &amp;  \begin{tabular}[c]{@{}r@{}}Población estándar\\ europea 1976\end{tabular}  &amp;  \begin{tabular}[c]{@{}r@{}}Población estándar\\ europea 2013\end{tabular}\\\hline</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="36.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="36.9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -2083,7 +1312,7 @@
         <v>\multicolumn{1}{|c|}{Grupo de edad}  &amp;  Población estándar mundial  &amp;  Población estándar europea 1976  &amp;  Población estándar europea 2013\\\hline</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C5" s="7" t="s">
         <v>37</v>
       </c>
@@ -2105,7 +1334,7 @@
         <v>0-4 años  &amp;  12.000  &amp;  8.000  &amp;  5.000\\</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C6" s="7" t="s">
         <v>38</v>
       </c>
@@ -2127,7 +1356,7 @@
         <v>5-9 años  &amp;  10.000  &amp;  7.000  &amp;  5.500\\</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C7" s="7" t="s">
         <v>39</v>
       </c>
@@ -2149,7 +1378,7 @@
         <v>10-14 años  &amp;  9.000  &amp;  7.000  &amp;  5.500\\</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C8" s="6" t="s">
         <v>40</v>
       </c>
@@ -2171,7 +1400,7 @@
         <v>15-19 años  &amp;  9.000  &amp;  7.000  &amp;  5.500\\</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C9" s="6" t="s">
         <v>41</v>
       </c>
@@ -2193,7 +1422,7 @@
         <v>20-24 años  &amp;  8.000  &amp;  7.000  &amp;  6.000\\</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C10" s="6" t="s">
         <v>42</v>
       </c>
@@ -2215,7 +1444,7 @@
         <v>25-29 años  &amp;  8.000  &amp;  7.000  &amp;  6.000\\</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C11" s="6" t="s">
         <v>43</v>
       </c>
@@ -2237,7 +1466,7 @@
         <v>30-34 años  &amp;  6.000  &amp;  7.000  &amp;  6.500\\</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C12" s="6" t="s">
         <v>44</v>
       </c>
@@ -2259,7 +1488,7 @@
         <v>35-39 años  &amp;  6.000  &amp;  7.000  &amp;  7.000\\</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C13" s="6" t="s">
         <v>45</v>
       </c>
@@ -2281,7 +1510,7 @@
         <v>40-44 años  &amp;  6.000  &amp;  7.000  &amp;  7.000\\</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C14" s="6" t="s">
         <v>46</v>
       </c>
@@ -2303,7 +1532,7 @@
         <v>45-49 años  &amp;  6.000  &amp;  7.000  &amp;  7.000\\</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C15" s="6" t="s">
         <v>47</v>
       </c>
@@ -2325,7 +1554,7 @@
         <v>50-54 años  &amp;  5.000  &amp;  7.000  &amp;  7.000\\</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C16" s="6" t="s">
         <v>48</v>
       </c>
@@ -2347,7 +1576,7 @@
         <v>55-59 años  &amp;  4.000  &amp;  6.000  &amp;  6.500\\</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C17" s="6" t="s">
         <v>49</v>
       </c>
@@ -2369,7 +1598,7 @@
         <v>60-64 años  &amp;  4.000  &amp;  5.000  &amp;  6.000\\</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C18" s="6" t="s">
         <v>50</v>
       </c>
@@ -2391,7 +1620,7 @@
         <v>65-69 años  &amp;  3.000  &amp;  4.000  &amp;  5.500\\</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C19" s="6" t="s">
         <v>51</v>
       </c>
@@ -2413,7 +1642,7 @@
         <v>70-74 años  &amp;  2.000  &amp;  3.000  &amp;  5.000\\</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C20" s="6" t="s">
         <v>52</v>
       </c>
@@ -2435,7 +1664,7 @@
         <v>75-79 años  &amp;  1.000  &amp;  2.000  &amp;  4.000\\</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C21" s="6" t="s">
         <v>53</v>
       </c>
@@ -2457,7 +1686,7 @@
         <v>80-84 años  &amp;  500  &amp;  1.000  &amp;  2.500\\</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -2482,7 +1711,7 @@
         <v>$\geq$85 años  &amp;  500  &amp;  1.000  &amp;  2.500\\\hline</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="24" x14ac:dyDescent="0.45">
       <c r="C25" s="8" t="s">
         <v>0</v>
       </c>
@@ -2496,7 +1725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C26" s="7" t="s">
         <v>20</v>
       </c>
@@ -2510,7 +1739,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C27" s="7" t="s">
         <v>4</v>
       </c>
@@ -2524,7 +1753,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C28" s="7" t="s">
         <v>5</v>
       </c>
@@ -2538,7 +1767,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C29" s="6" t="s">
         <v>6</v>
       </c>
@@ -2552,7 +1781,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C30" s="6" t="s">
         <v>7</v>
       </c>
@@ -2566,7 +1795,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C31" s="6" t="s">
         <v>8</v>
       </c>
@@ -2580,7 +1809,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C32" s="6" t="s">
         <v>9</v>
       </c>
@@ -2594,7 +1823,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C33" s="6" t="s">
         <v>10</v>
       </c>
@@ -2608,7 +1837,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C34" s="6" t="s">
         <v>11</v>
       </c>
@@ -2622,7 +1851,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C35" s="6" t="s">
         <v>12</v>
       </c>
@@ -2636,7 +1865,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C36" s="6" t="s">
         <v>13</v>
       </c>
@@ -2650,7 +1879,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C37" s="6" t="s">
         <v>14</v>
       </c>
@@ -2664,7 +1893,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C38" s="6" t="s">
         <v>15</v>
       </c>
@@ -2678,7 +1907,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C39" s="6" t="s">
         <v>16</v>
       </c>
@@ -2692,7 +1921,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C40" s="6" t="s">
         <v>17</v>
       </c>
@@ -2706,7 +1935,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C41" s="6" t="s">
         <v>18</v>
       </c>
@@ -2720,7 +1949,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C42" s="6" t="s">
         <v>19</v>
       </c>
@@ -2734,7 +1963,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C43" s="6" t="s">
         <v>21</v>
       </c>
@@ -2765,18 +1994,18 @@
       <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2809,7 +2038,7 @@
         <v>Sexo &amp; Población &amp; Fuente &amp; N &amp; TB &amp; TE-W &amp; TE-oE &amp; TE-nE\\\hline</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>77</v>
       </c>
@@ -2835,7 +2064,7 @@
         <v>\multirow{3}{*}{Hombres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 8.818.685 &amp; 229,0 &amp; 204,7 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B7" s="12"/>
       <c r="C7" s="21" t="s">
         <v>76</v>
@@ -2863,7 +2092,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 2.059.673 &amp; 572,9 &amp; 302,7 &amp; 436,0 &amp; 651,7\\</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2894,7 +2123,7 @@
         <v xml:space="preserve"> &amp; España &amp; ECIS \cite{ECIS} &amp; 142.353 &amp; 625,6 &amp; 309,7 &amp; 444,7 &amp; 658,6\\\hline</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>78</v>
       </c>
@@ -2920,7 +2149,7 @@
         <v>\multirow{3}{*}{Mujeres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 8.218.216 &amp; 217,3 &amp; 175,6 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C10" s="21" t="s">
         <v>76</v>
       </c>
@@ -2947,7 +2176,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 1.851.644 &amp; 481,8 &amp; 242,7 &amp; 332,6 &amp; 451,2\\</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -2977,7 +2206,7 @@
         <v xml:space="preserve"> &amp; España &amp; ECIS \cite{ECIS} &amp; 106.647 &amp; 451,1 &amp; 218,4 &amp; 298,5 &amp; 401,7\\\hline</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>79</v>
       </c>
@@ -3003,7 +2232,7 @@
         <v>\multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; GCO \cite{GCO} &amp; 17.036.901 &amp; 223,2 &amp; 187,8 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C13" s="21" t="s">
         <v>76</v>
       </c>
@@ -3030,7 +2259,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 3.911.317 &amp; 525,8 &amp; 266,7 &amp; 374,3 &amp; 531,9\\</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -3060,7 +2289,7 @@
         <v xml:space="preserve"> &amp; España &amp; ECIS \cite{ECIS} &amp; 249.000 &amp; 536,7 &amp; 259,4 &amp; 363,8 &amp; 515,3\\\hline</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>58</v>
       </c>
@@ -3068,7 +2297,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="13">
         <v>8818685</v>
       </c>
@@ -3089,7 +2318,7 @@
         <v>8.818.685</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22" s="14">
         <v>2059673</v>
       </c>
@@ -3110,7 +2339,7 @@
         <v>2.059.673</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="15">
         <v>142353</v>
       </c>
@@ -3128,7 +2357,7 @@
         <v>142.353</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="16">
         <v>8218216</v>
       </c>
@@ -3149,7 +2378,7 @@
         <v>8.218.216</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" s="14">
         <v>1851644</v>
       </c>
@@ -3170,7 +2399,7 @@
         <v>1.851.644</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="14">
         <v>106647</v>
       </c>
@@ -3188,7 +2417,7 @@
         <v>106.647</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="16">
         <v>17036901</v>
       </c>
@@ -3209,7 +2438,7 @@
         <v>17.036.901</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28" s="14">
         <v>3911317</v>
       </c>
@@ -3230,7 +2459,7 @@
         <v>3.911.317</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29" s="16">
         <v>249000</v>
       </c>
@@ -3262,18 +2491,18 @@
       <selection activeCell="G5" sqref="G5:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -3306,7 +2535,7 @@
         <v>Sexo &amp; Población &amp; Fuente &amp; N &amp; TB &amp; TE-W &amp; TE-oE &amp; TE-nE\\\hline</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>77</v>
       </c>
@@ -3332,7 +2561,7 @@
         <v>\multirow{3}{*}{Hombres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 596.574 &amp; 15,5 &amp; 13,9 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B7" s="12"/>
       <c r="C7" s="21" t="s">
         <v>76</v>
@@ -3360,7 +2589,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 55.825 &amp; 15,5 &amp; 8,0 &amp; 11,7 &amp; 17,7\\</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -3391,7 +2620,7 @@
         <v xml:space="preserve"> &amp; España &amp; ECIS \cite{ECIS} &amp; 4.976 &amp; 21,9 &amp; 10,9 &amp; 15,7 &amp; 22,5\\\hline</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>78</v>
       </c>
@@ -3417,7 +2646,7 @@
         <v>\multirow{3}{*}{Mujeres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 244.506 &amp; 6,5 &amp; 4,9 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C10" s="21" t="s">
         <v>76</v>
       </c>
@@ -3444,7 +2673,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 26.641 &amp; 6,9 &amp; 2,7 &amp; 4,0 &amp; 6,3\\</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -3474,7 +2703,7 @@
         <v xml:space="preserve"> &amp; España &amp; ECIS \cite{ECIS} &amp; 1.654 &amp; 7,0 &amp; 2,4 &amp; 3,6 &amp; 6,0\\\hline</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>79</v>
       </c>
@@ -3500,7 +2729,7 @@
         <v>\multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; GCO \cite{GCO} &amp; 841.080 &amp; 11,0 &amp; 9,3 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C13" s="21" t="s">
         <v>76</v>
       </c>
@@ -3527,7 +2756,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 82.466 &amp; 11,1 &amp; 5,1 &amp; 7,4 &amp; 11,3\\</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -3557,7 +2786,7 @@
         <v xml:space="preserve"> &amp; España &amp; ECIS \cite{ECIS} &amp; 6.630 &amp; 14,3 &amp; 6,5 &amp; 9,3 &amp; 13,6\\\hline</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>58</v>
       </c>
@@ -3565,7 +2794,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="13">
         <v>596574</v>
       </c>
@@ -3583,7 +2812,7 @@
         <v>596.574</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22" s="23">
         <v>55825</v>
       </c>
@@ -3601,7 +2830,7 @@
         <v>55.825</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="15">
         <v>4976</v>
       </c>
@@ -3619,7 +2848,7 @@
         <v>4.976</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="16">
         <v>244506</v>
       </c>
@@ -3637,7 +2866,7 @@
         <v>244.506</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" s="24">
         <v>26641</v>
       </c>
@@ -3655,7 +2884,7 @@
         <v>26.641</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="25">
         <v>1654</v>
       </c>
@@ -3673,7 +2902,7 @@
         <v>1.654</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="16">
         <v>841080</v>
       </c>
@@ -3691,7 +2920,7 @@
         <v>841.080</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28" s="26">
         <v>82466</v>
       </c>
@@ -3709,7 +2938,7 @@
         <v>82.466</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29" s="16">
         <v>6630</v>
       </c>
@@ -3740,18 +2969,18 @@
       <selection activeCell="G5" sqref="G5:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -3784,7 +3013,7 @@
         <v>Sexo &amp; Población &amp; Fuente &amp; N &amp; TB &amp; TE-W &amp; TE-oE &amp; TE-nE\\\hline</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>77</v>
       </c>
@@ -3810,7 +3039,7 @@
         <v>\multirow{3}{*}{Hombres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 1.026.215 &amp; 26,6 &amp; 23,6 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B7" s="12"/>
       <c r="C7" s="21" t="s">
         <v>76</v>
@@ -3838,7 +3067,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 275.519 &amp; 76,6 &amp; 38,1 &amp; 56,8 &amp; 88,9\\</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -3869,7 +3098,7 @@
         <v xml:space="preserve"> &amp; España &amp; ECIS \cite{ECIS} &amp; 23.013 &amp; 101,1 &amp; 45,8 &amp; 68,5 &amp; 107,2\\\hline</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>78</v>
       </c>
@@ -3895,7 +3124,7 @@
         <v>\multirow{3}{*}{Mujeres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 823.303 &amp; 21,8 &amp; 16,3 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C10" s="21" t="s">
         <v>76</v>
       </c>
@@ -3922,7 +3151,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 236.101 &amp; 61,4 &amp; 25,2 &amp; 37,0 &amp; 56,3\\</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -3952,7 +3181,7 @@
         <v xml:space="preserve"> &amp; España &amp; ECIS \cite{ECIS} &amp; 14.642 &amp; 61,9 &amp; 23,6 &amp; 34,9 &amp; 53,5\\\hline</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>79</v>
       </c>
@@ -3978,7 +3207,7 @@
         <v>\multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; GCO \cite{GCO} &amp; 1.849.518 &amp; 24,2 &amp; 19,7 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C13" s="21" t="s">
         <v>76</v>
       </c>
@@ -4005,7 +3234,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 511.620 &amp; 68,8 &amp; 30,8 &amp; 45,6 &amp; 70,0\\</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -4035,7 +3264,7 @@
         <v xml:space="preserve"> &amp; España &amp; ECIS \cite{ECIS} &amp; 37.655 &amp; 81,1 &amp; 33,9 &amp; 50,4 &amp; 77,5\\\hline</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>58</v>
       </c>
@@ -4043,7 +3272,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="13">
         <v>1026215</v>
       </c>
@@ -4055,7 +3284,7 @@
         <v>.</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22" s="14">
         <v>275519</v>
       </c>
@@ -4067,7 +3296,7 @@
         <v>.</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="15">
         <v>23013</v>
       </c>
@@ -4079,7 +3308,7 @@
         <v>.</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="16">
         <v>823303</v>
       </c>
@@ -4091,7 +3320,7 @@
         <v>.</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" s="15">
         <v>236101</v>
       </c>
@@ -4103,7 +3332,7 @@
         <v>.</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="15">
         <v>14642</v>
       </c>
@@ -4115,7 +3344,7 @@
         <v>.</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="16">
         <v>1849518</v>
       </c>
@@ -4127,7 +3356,7 @@
         <v>.</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28" s="15">
         <v>511620</v>
       </c>
@@ -4139,7 +3368,7 @@
         <v>.</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29" s="15">
         <v>37655</v>
       </c>
@@ -4164,18 +3393,18 @@
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -4208,7 +3437,7 @@
         <v>Sexo &amp; Población &amp; Fuente &amp; N &amp; TB &amp; TE-W &amp; TE-oE &amp; TE-nE\\\hline</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>77</v>
       </c>
@@ -4234,7 +3463,7 @@
         <v>\multirow{3}{*}{Hombres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 5.347.295 &amp; 138,9 &amp; 121,9 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B7" s="12"/>
       <c r="C7" s="21" t="s">
         <v>76</v>
@@ -4262,7 +3491,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 1.077.986 &amp; 299,8 &amp; 143,2 &amp; 217,4 &amp; 355,4\\</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4293,7 +3522,7 @@
         <v xml:space="preserve"> &amp; España &amp; MSCBS \cite{MSCBS} &amp; 65.610 &amp; 286,4 &amp; 121,3 &amp; 186,8 &amp; 314,1\\\hline</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>78</v>
       </c>
@@ -4319,7 +3548,7 @@
         <v>\multirow{3}{*}{Mujeres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 4.142.577 &amp; 109,5 &amp; 82,7 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C10" s="21" t="s">
         <v>76</v>
       </c>
@@ -4346,7 +3575,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 851.723 &amp; 221,6 &amp; 86,4 &amp; 128,1 &amp; 201,0\\</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -4376,7 +3605,7 @@
         <v xml:space="preserve"> &amp; España &amp; MSCBS \cite{MSCBS} &amp; 42.248 &amp; 177,4 &amp; 63,2 &amp; 94,6 &amp; 151,1\\\hline</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>79</v>
       </c>
@@ -4402,7 +3631,7 @@
         <v>\multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; GCO \cite{GCO} &amp; 9.489.872 &amp; 124,3 &amp; 100,5 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C13" s="21" t="s">
         <v>76</v>
       </c>
@@ -4429,7 +3658,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 1.929.709 &amp; 259,4 &amp; 110,8 &amp; 165,8 &amp; 263,9\\</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -4459,7 +3688,7 @@
         <v xml:space="preserve"> &amp; España &amp; MSCBS \cite{MSCBS} &amp; 107.858 &amp; 230,8 &amp; 89,4 &amp; 135,4 &amp; 221,2\\\hline</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>58</v>
       </c>
@@ -4467,7 +3696,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="18">
         <v>5347295</v>
       </c>
@@ -4488,7 +3717,7 @@
         <v>5.347.295</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22" s="18">
         <v>1077986</v>
       </c>
@@ -4509,7 +3738,7 @@
         <v>1.077.986</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="18">
         <v>65610</v>
       </c>
@@ -4527,7 +3756,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="18">
         <v>4142577</v>
       </c>
@@ -4548,7 +3777,7 @@
         <v>4.142.577</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" s="18">
         <v>851723</v>
       </c>
@@ -4569,7 +3798,7 @@
         <v>0.851.723</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="18">
         <v>42248</v>
       </c>
@@ -4587,7 +3816,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="18">
         <v>9489872</v>
       </c>
@@ -4608,7 +3837,7 @@
         <v>9.489.872</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28" s="19">
         <v>1929709</v>
       </c>
@@ -4629,7 +3858,7 @@
         <v>1.929.709</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29" s="18" t="s">
         <v>111</v>
       </c>
@@ -4661,18 +3890,18 @@
       <selection activeCell="G5" sqref="G5:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -4705,7 +3934,7 @@
         <v>Sexo &amp; Población &amp; Fuente &amp; N &amp; TB &amp; TE-W &amp; TE-oE &amp; TE-nE\\\hline</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>77</v>
       </c>
@@ -4731,7 +3960,7 @@
         <v>\multirow{3}{*}{Hombres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 548.375 &amp; 14,2 &amp; 12,7 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B7" s="12"/>
       <c r="C7" s="21" t="s">
         <v>76</v>
@@ -4759,7 +3988,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 50.365 &amp; 14,0 &amp; 6,8 &amp; 10,3 &amp; 16,4\\</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4790,7 +4019,7 @@
         <v xml:space="preserve"> &amp; España &amp; MSCBS \cite{MSCBS} &amp; 3.577 &amp; 15,6 &amp; 7,0 &amp; 10,7 &amp; 17,0\\\hline</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>78</v>
       </c>
@@ -4816,7 +4045,7 @@
         <v>\multirow{3}{*}{Mujeres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 233.256 &amp; 6,2 &amp; 4,6 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C10" s="21" t="s">
         <v>76</v>
       </c>
@@ -4843,7 +4072,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 27.010 &amp; 7,0 &amp; 2,4 &amp; 3,8 &amp; 6,3\\</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -4873,7 +4102,7 @@
         <v xml:space="preserve"> &amp; España &amp; MSCBS \cite{MSCBS} &amp; 1.564 &amp; 6,6 &amp; 2,0 &amp; 3,2 &amp; 5,6\\\hline</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>79</v>
       </c>
@@ -4899,7 +4128,7 @@
         <v>\multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; GCO \cite{GCO} &amp; 781.631 &amp; 10,2 &amp; 8,5 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C13" s="21" t="s">
         <v>76</v>
       </c>
@@ -4926,7 +4155,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 77.375 &amp; 10,4 &amp; 4,4 &amp; 6,6 &amp; 10,6\\</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -4956,7 +4185,7 @@
         <v xml:space="preserve"> &amp; España &amp; MSCBS \cite{MSCBS} &amp; 5.141 &amp; 11,0 &amp; 4,4 &amp; 6,7 &amp; 10,7\\\hline</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>58</v>
       </c>
@@ -4964,7 +4193,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="18"/>
       <c r="C21" s="11">
         <f>QUOTIENT(B21,1000000)</f>
@@ -4983,7 +4212,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22" s="18"/>
       <c r="C22" s="11">
         <f t="shared" ref="C22:C28" si="4">QUOTIENT(B22,1000000)</f>
@@ -5002,7 +4231,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="18"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="e">
@@ -5018,7 +4247,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="18"/>
       <c r="C24" s="11">
         <f t="shared" si="4"/>
@@ -5037,7 +4266,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" s="18"/>
       <c r="C25" s="11">
         <f t="shared" si="4"/>
@@ -5056,7 +4285,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="18"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="e">
@@ -5072,7 +4301,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="18"/>
       <c r="C27" s="11">
         <f t="shared" si="4"/>
@@ -5091,7 +4320,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28" s="19"/>
       <c r="C28" s="11">
         <f t="shared" si="4"/>
@@ -5110,7 +4339,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29" s="18"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="e">
@@ -5140,18 +4369,18 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.9140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.92578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -5184,7 +4413,7 @@
         <v>Sexo &amp; Población &amp; Fuente &amp; N &amp; TB &amp; TE-W &amp; TE-oE &amp; TE-nE\\\hline</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>77</v>
       </c>
@@ -5210,7 +4439,7 @@
         <v>\multirow{3}{*}{Hombres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 484.224 &amp; 12,6 &amp; 10,8 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B7" s="12"/>
       <c r="C7" s="21" t="s">
         <v>76</v>
@@ -5238,7 +4467,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 131.155 &amp; 36,5 &amp; 16,4 &amp; 25,7 &amp; 44,3\\</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5269,7 +4498,7 @@
         <v xml:space="preserve"> &amp; España &amp; MSCBS \cite{MSCBS} &amp; 9.222 &amp; 40,3 &amp; 15,8 &amp; 25,1 &amp; 44,4\\\hline</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>78</v>
       </c>
@@ -5295,7 +4524,7 @@
         <v>\multirow{3}{*}{Mujeres} &amp; Mundo &amp; GCO \cite{GCO} &amp; 396.568 &amp; 10,5 &amp; 7,2 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C10" s="21" t="s">
         <v>76</v>
       </c>
@@ -5322,7 +4551,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 115.059 &amp; 29,9 &amp; 10,0 &amp; 15,6 &amp; 26,6\\</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -5352,7 +4581,7 @@
         <v xml:space="preserve"> &amp; España &amp; MSCBS \cite{MSCBS} &amp; 6.066 &amp; 25,5 &amp; 7,5 &amp; 11,9 &amp; 20,7\\\hline</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>79</v>
       </c>
@@ -5378,7 +4607,7 @@
         <v>\multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; GCO \cite{GCO} &amp; 880.792 &amp; 11,5 &amp; 8,9 &amp;  &amp; \\</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C13" s="21" t="s">
         <v>76</v>
       </c>
@@ -5405,7 +4634,7 @@
         <v xml:space="preserve"> &amp; Europa &amp; ECIS \cite{ECIS} &amp; 246.214 &amp; 33,1 &amp; 12,8 &amp; 19,9 &amp; 33,8\\</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -5435,7 +4664,7 @@
         <v xml:space="preserve"> &amp; España &amp; MSCBS \cite{MSCBS} &amp; 15.288 &amp; 32,7 &amp; 11,2 &amp; 17,7 &amp; 30,9\\\hline</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>58</v>
       </c>
@@ -5443,7 +4672,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="18"/>
       <c r="C21" s="11">
         <f>QUOTIENT(B21,1000000)</f>
@@ -5462,7 +4691,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22" s="18"/>
       <c r="C22" s="11">
         <f t="shared" ref="C22:C28" si="4">QUOTIENT(B22,1000000)</f>
@@ -5481,7 +4710,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="18"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="e">
@@ -5497,7 +4726,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="18"/>
       <c r="C24" s="11">
         <f t="shared" si="4"/>
@@ -5516,7 +4745,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" s="18"/>
       <c r="C25" s="11">
         <f t="shared" si="4"/>
@@ -5535,7 +4764,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="18"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="e">
@@ -5551,7 +4780,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="18"/>
       <c r="C27" s="11">
         <f t="shared" si="4"/>
@@ -5570,7 +4799,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28" s="19"/>
       <c r="C28" s="11">
         <f t="shared" si="4"/>
@@ -5589,7 +4818,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29" s="18"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="e">
@@ -5611,22 +4840,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82833DD-B50C-4E21-A8FA-CE9B4A74514D}">
-  <dimension ref="A3:L28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B244C3-CB16-495F-980A-6CB4471F2FAB}">
+  <dimension ref="A3:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="54.08203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.2109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>152</v>
       </c>
@@ -5634,13 +4862,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="9"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -5651,29 +4885,26 @@
         <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>211</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>216</v>
+        <v>147</v>
       </c>
       <c r="H5" t="s">
-        <v>217</v>
+        <v>56</v>
       </c>
       <c r="I5" t="s">
-        <v>223</v>
-      </c>
-      <c r="J5" t="s">
-        <v>224</v>
-      </c>
-      <c r="L5" s="9" t="str">
-        <f xml:space="preserve"> C5 &amp; " &amp; " &amp; D5 &amp; " &amp; " &amp; E5  &amp; " &amp; " &amp; G5 &amp; " &amp; " &amp; H5 &amp; " &amp; " &amp; I5 &amp; " &amp; " &amp; J5 &amp; "\\" &amp; IF(B5="x","\hline","")</f>
-        <v>Localización &amp; Sexo &amp; Población y año &amp; Sup obs 1 año &amp; Sup rel 1 año &amp; Sup obs 5 año &amp; Sup rel 5 año\\\hline</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+      <c r="K5" s="9" t="str">
+        <f xml:space="preserve"> C5 &amp; " &amp; " &amp; D5 &amp; " &amp; " &amp; E5  &amp; " &amp; " &amp; F5 &amp; " &amp; " &amp; G5 &amp; " &amp; " &amp; H5 &amp; " &amp; " &amp; I5 &amp; "\\" &amp; IF(B5="x","\hline","")</f>
+        <v>Localización &amp; Sexo &amp; Población &amp; N &amp; Tasa &amp; N &amp; Tasa\\\hline</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>146</v>
       </c>
@@ -5681,361 +4912,632 @@
         <v>77</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="L6" s="9" t="str">
-        <f xml:space="preserve"> C6 &amp; " &amp; " &amp; D6 &amp; " &amp; " &amp; E6  &amp; " &amp; " &amp; G6 &amp; " &amp; " &amp; H6 &amp; " &amp; " &amp; I6 &amp; " &amp; " &amp; J6 &amp; "\\" &amp; IF(B6="x"," \hline","") &amp; IF(A6="x"," \cline{2-7}","")</f>
-        <v>\multirow{9}{*}{Total del cáncer EPNM} &amp; \multirow{3}{*}{Hombres} &amp; \begin{tabular}[c]{@{}c@{}}Mundo\\(años)\end{tabular} &amp;  &amp;  &amp;  &amp; existe\\</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="G6" s="31">
+        <v>145.6</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="I6" s="31">
+        <v>464.7</v>
+      </c>
+      <c r="K6" s="9" t="str">
+        <f xml:space="preserve"> C6 &amp; " &amp; " &amp; D6 &amp; " &amp; " &amp; E6  &amp; " &amp; " &amp; F6 &amp; " &amp; " &amp; G6 &amp; " &amp; " &amp; H6 &amp; " &amp; " &amp; I6 &amp; "\\" &amp; IF(B6="x"," \hline","") &amp; IF(A6="x"," \cline{2-7}","")</f>
+        <v>\multirow{9}{*}{Total del cáncer EPNM} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 5.607.801 &amp; 145,6 &amp; 17.895.356 &amp; 464,7\\</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D7" s="12"/>
       <c r="E7" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>218</v>
+        <v>76</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="31">
+        <v>418.4</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="J7" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="L7" s="9" t="str">
-        <f t="shared" ref="L7:L23" si="0" xml:space="preserve"> C7 &amp; " &amp; " &amp; D7 &amp; " &amp; " &amp; E7  &amp; " &amp; " &amp; G7 &amp; " &amp; " &amp; H7 &amp; " &amp; " &amp; I7 &amp; " &amp; " &amp; J7 &amp; "\\" &amp; IF(B7="x"," \hline","") &amp; IF(A7="x"," \cline{2-7}","")</f>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp; existe &amp; existe &amp; existe &amp; existe\\</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>209</v>
+      </c>
+      <c r="I7" s="31">
+        <v>1414.7</v>
+      </c>
+      <c r="K7" s="9" t="str">
+        <f t="shared" ref="K7:K32" si="0" xml:space="preserve"> C7 &amp; " &amp; " &amp; D7 &amp; " &amp; " &amp; E7  &amp; " &amp; " &amp; F7 &amp; " &amp; " &amp; G7 &amp; " &amp; " &amp; H7 &amp; " &amp; " &amp; I7 &amp; "\\" &amp; IF(B7="x"," \hline","") &amp; IF(A7="x"," \cline{2-7}","")</f>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 1.504.232 &amp; 418,4 &amp; 5.086.515 &amp; 1414,7\\</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="G8" s="31"/>
+        <v>69</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>153</v>
+      </c>
       <c r="H8" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="I8" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="L8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp; existe &amp; existe &amp; existe\\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+      <c r="I8" s="31">
+        <v>1566.3</v>
+      </c>
+      <c r="K8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 105.599 &amp; 464,0 &amp; 356.427 &amp; 1566,3\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>78</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="L9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp;  &amp;  &amp;  &amp; \\</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F9" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="G9" s="31">
+        <v>150.4</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="I9" s="31">
+        <v>548.29999999999995</v>
+      </c>
+      <c r="K9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 5.688.175 &amp; 150,4 &amp; 20.738.064 &amp; 548,3\\</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E10" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="L10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" s="31">
+        <v>373.4</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="I10" s="31">
+        <v>1409.8</v>
+      </c>
+      <c r="K10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 1.434.849 &amp; 373,4 &amp; 5.417.680 &amp; 1409,8\\</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="L11" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
-        <v>145</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="I11" s="31">
+        <v>1363.5</v>
+      </c>
+      <c r="K11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 84.409 &amp; 357,0 &amp; 322.341 &amp; 1363,5\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="L12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>\multirow{9}{*}{Hígado} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp;  &amp;  &amp;  &amp; \\</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D13" s="12"/>
+      <c r="F12" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="I12" s="31">
+        <v>506.1</v>
+      </c>
+      <c r="K12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 11.295.976 &amp; 148,0 &amp; 38.633.420 &amp; 506,1\\</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E13" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="L13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="G13" s="31">
+        <v>395.1</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="I13" s="31">
+        <v>1412.2</v>
+      </c>
+      <c r="K13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 2.939.081 &amp; 395,1 &amp; 10.504.195 &amp; 1412,2\\</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="12"/>
       <c r="E14" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="L14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="G14" s="31">
+        <v>409.5</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="I14" s="31">
+        <v>1462.9</v>
+      </c>
+      <c r="K14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 190.008 &amp; 409,5 &amp; 678.768 &amp; 1462,9\\ \hline</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C15" t="s">
+        <v>145</v>
+      </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="L15" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp;  &amp;  &amp;  &amp; \\</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F15" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="G15" s="32">
+        <v>6.1</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="I15" s="32">
+        <v>12.2</v>
+      </c>
+      <c r="K15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>\multirow{9}{*}{Hígado} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 236.669 &amp; 6,1 &amp; 471.525 &amp; 12,2\\</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="D16" s="12"/>
       <c r="E16" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="L16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="G16" s="33">
+        <v>5.9</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="I16" s="32">
+        <v>11.1</v>
+      </c>
+      <c r="K16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 21.240 &amp; 5,9 &amp; 39.867 &amp; 11,1\\</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>23</v>
       </c>
+      <c r="D17" s="12"/>
       <c r="E17" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="L17" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C18" t="s">
-        <v>150</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="G17" s="33">
+        <v>8.5</v>
+      </c>
+      <c r="H17" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="I17" s="33">
+        <v>15.9</v>
+      </c>
+      <c r="K17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 1.924 &amp; 8,5 &amp; 3.618 &amp; 15,9\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="L18" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>\multirow{9}{*}{Colon-recto} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp;  &amp;  &amp;  &amp; \\</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D19" s="12"/>
+      <c r="F18" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="G18" s="32">
+        <v>2.6</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="I18" s="32">
+        <v>5.4</v>
+      </c>
+      <c r="K18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 97.621 &amp; 2,6 &amp; 203.685 &amp; 5,4\\</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E19" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="L19" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="G19" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="I19" s="32">
+        <v>4.8</v>
+      </c>
+      <c r="K19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 9.719 &amp; 2,5 &amp; 18.610 &amp; 4,8\\</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="12"/>
       <c r="E20" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="L20" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+      <c r="F20" s="33">
+        <v>580</v>
+      </c>
+      <c r="G20" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="H20" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="I20" s="33">
+        <v>4.7</v>
+      </c>
+      <c r="K20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 580 &amp; 2,5 &amp; 1.102 &amp; 4,7\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="L21" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp;  &amp;  &amp;  &amp; \\</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F21" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="G21" s="32">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="I21" s="32">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 334.290 &amp; 4,4 &amp; 675.210 &amp; 8,8\\</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E22" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="L22" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}Europa\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="G22" s="33">
+        <v>4.2</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="I22" s="32">
+        <v>7.9</v>
+      </c>
+      <c r="K22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 30.959 &amp; 4,2 &amp; 58.477 &amp; 7,9\\</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="F23" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="L23" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> &amp;  &amp; \begin{tabular}[c]{@{}c@{}}España\\(2000-2007)\end{tabular} &amp;  &amp;  &amp;  &amp; \\ \cline{2-7}</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E27" s="35" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E28" s="34" t="s">
-        <v>220</v>
+        <v>69</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="G23" s="33">
+        <v>5.4</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="I23" s="33">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 2.504 &amp; 5,4 &amp; 4.720 &amp; 10,2\\ \hline</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" s="32">
+        <v>19.5</v>
+      </c>
+      <c r="H24" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="I24" s="32">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="K24" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>\multirow{9}{*}{Colon-recto} &amp; \multirow{3}{*}{Hombres} &amp; Mundo &amp; 749.774 &amp; 19,5 &amp; 2.595.326 &amp; 67,4\\</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="D25" s="12"/>
+      <c r="E25" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="G25" s="33">
+        <v>59.3</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="I25" s="32">
+        <v>208.2</v>
+      </c>
+      <c r="K25" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 213.233 &amp; 59,3 &amp; 748.455 &amp; 208,2\\</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="G26" s="33">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="H26" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="I26" s="33">
+        <v>279.5</v>
+      </c>
+      <c r="K26" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 18.059 &amp; 79,4 &amp; 63.593 &amp; 279,5\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="K27" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{Mujeres} &amp; Mundo &amp; 606.377 &amp; 16,0 &amp; 2.194.309 &amp; 58,0\\</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E28" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="G28" s="33">
+        <v>46.6</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="I28" s="32">
+        <v>170.6</v>
+      </c>
+      <c r="K28" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 178.969 &amp; 46,6 &amp; 655.422 &amp; 170,6\\</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="G29" s="33">
+        <v>48.5</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="I29" s="33">
+        <v>178.2</v>
+      </c>
+      <c r="K29" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 11.463 &amp; 48,5 &amp; 42.121 &amp; 178,2\\ \cline{2-7}</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="G30" s="32">
+        <v>17.8</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="I30" s="32">
+        <v>62.8</v>
+      </c>
+      <c r="K30" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp; \multirow{3}{*}{\begin{tabular}[c]{@{}c@{}}Ambos\\sexos\end{tabular}} &amp; Mundo &amp; 1.356.151 &amp; 17,8 &amp; 4.789.635 &amp; 62,8\\</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E31" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="G31" s="33">
+        <v>52.7</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="I31" s="32">
+        <v>188.7</v>
+      </c>
+      <c r="K31" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; Europa &amp; 392.202 &amp; 52,7 &amp; 1.403.877 &amp; 188,7\\</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="G32" s="33">
+        <v>63.6</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="I32" s="33">
+        <v>227.8</v>
+      </c>
+      <c r="K32" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &amp;  &amp; España &amp; 29.522 &amp; 63,6 &amp; 105.714 &amp; 227,8\\ \hline</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizar con datos clínicos hígado
</commit_message>
<xml_diff>
--- a/Documento/tablas/tablas_tfm.xlsx
+++ b/Documento/tablas/tablas_tfm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Dropbox/Transporte_interno/Máster/Ciencia de Datos/TFM/Documento/tablas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6536E978-8705-5248-8EE1-913E5CEA9508}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BD59B3-6948-2C47-B357-0CE4E5E6D09C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13180" yWindow="2140" windowWidth="21340" windowHeight="17920" tabRatio="752" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12260" yWindow="2140" windowWidth="21340" windowHeight="17920" tabRatio="752" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="248">
   <si>
     <t>Grupo de edad</t>
   </si>
@@ -779,6 +779,15 @@
   </si>
   <si>
     <t>&lt;0.001</t>
+  </si>
+  <si>
+    <t>404 (100%)</t>
+  </si>
+  <si>
+    <t>Número de casos (Porcentaje)</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -925,7 +934,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1023,10 +1032,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1376,41 +1388,56 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056BCBA3-1777-4443-88F8-AEA97B8D4F5E}">
-  <dimension ref="B2:D34"/>
+  <dimension ref="B2:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.83203125" style="36"/>
+    <col min="6" max="6" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C2" s="36" t="s">
         <v>56</v>
       </c>
       <c r="D2" s="36" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="G2" s="40" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="34" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="C3" s="36">
         <v>404</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F3" s="34" t="s">
+        <v>247</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="38" t="s">
         <v>55</v>
       </c>
       <c r="D4" s="37"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F4" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="35"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="35" t="s">
         <v>225</v>
       </c>
@@ -1421,8 +1448,15 @@
         <f>C5/$C$3</f>
         <v>0.65346534653465349</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F5" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="G5" s="35" t="str">
+        <f>C5 &amp; " (" &amp; ROUND(100*D5,1) &amp; "%)"</f>
+        <v>264 (65,3%)</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="35" t="s">
         <v>226</v>
       </c>
@@ -1433,14 +1467,25 @@
         <f>C6/$C$3</f>
         <v>0.34653465346534651</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F6" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="G6" s="35" t="str">
+        <f>C6 &amp; " (" &amp; ROUND(100*D6,1) &amp; "%)"</f>
+        <v>140 (34,7%)</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="38" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="37"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F7" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="35"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="35" t="s">
         <v>219</v>
       </c>
@@ -1448,11 +1493,18 @@
         <v>34</v>
       </c>
       <c r="D8" s="37">
-        <f>C8/$C$3</f>
+        <f t="shared" ref="D8:D14" si="0">C8/$C$3</f>
         <v>8.4158415841584164E-2</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F8" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="G8" s="35" t="str">
+        <f t="shared" ref="G7:G34" si="1">C8 &amp; " (" &amp; ROUND(100*D8,1) &amp; "%)"</f>
+        <v>34 (8,4%)</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="35" t="s">
         <v>220</v>
       </c>
@@ -1460,11 +1512,18 @@
         <v>40</v>
       </c>
       <c r="D9" s="37">
-        <f>C9/$C$3</f>
+        <f t="shared" si="0"/>
         <v>9.9009900990099015E-2</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F9" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="G9" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>40 (9,9%)</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="35" t="s">
         <v>221</v>
       </c>
@@ -1472,11 +1531,18 @@
         <v>106</v>
       </c>
       <c r="D10" s="37">
-        <f>C10/$C$3</f>
+        <f t="shared" si="0"/>
         <v>0.26237623762376239</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F10" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="G10" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>106 (26,2%)</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="35" t="s">
         <v>222</v>
       </c>
@@ -1484,11 +1550,18 @@
         <v>127</v>
       </c>
       <c r="D11" s="37">
-        <f>C11/$C$3</f>
+        <f t="shared" si="0"/>
         <v>0.31435643564356436</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F11" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="G11" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>127 (31,4%)</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="35" t="s">
         <v>223</v>
       </c>
@@ -1496,11 +1569,18 @@
         <v>77</v>
       </c>
       <c r="D12" s="37">
-        <f>C12/$C$3</f>
+        <f t="shared" si="0"/>
         <v>0.1905940594059406</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F12" s="35" t="s">
+        <v>223</v>
+      </c>
+      <c r="G12" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>77 (19,1%)</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="35" t="s">
         <v>224</v>
       </c>
@@ -1508,11 +1588,18 @@
         <v>16</v>
       </c>
       <c r="D13" s="37">
-        <f>C13/$C$3</f>
+        <f t="shared" si="0"/>
         <v>3.9603960396039604E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F13" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="G13" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>16 (4%)</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="35" t="s">
         <v>217</v>
       </c>
@@ -1520,16 +1607,27 @@
         <v>4</v>
       </c>
       <c r="D14" s="37">
-        <f>C14/$C$3</f>
+        <f t="shared" si="0"/>
         <v>9.9009900990099011E-3</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F14" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="G14" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>4 (1%)</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="34" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F15" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="G15" s="35"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="35" t="s">
         <v>213</v>
       </c>
@@ -1540,8 +1638,15 @@
         <f>C16/$C$3</f>
         <v>0.46782178217821785</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F16" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="G16" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>189 (46,8%)</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="35" t="s">
         <v>215</v>
       </c>
@@ -1549,11 +1654,18 @@
         <v>95</v>
       </c>
       <c r="D17" s="37">
-        <f t="shared" ref="D17:D34" si="0">C17/$C$3</f>
+        <f t="shared" ref="D17:D34" si="2">C17/$C$3</f>
         <v>0.23514851485148514</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F17" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="G17" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>95 (23,5%)</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="35" t="s">
         <v>216</v>
       </c>
@@ -1561,11 +1673,18 @@
         <v>82</v>
       </c>
       <c r="D18" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.20297029702970298</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F18" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="G18" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>82 (20,3%)</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="35" t="s">
         <v>214</v>
       </c>
@@ -1573,11 +1692,18 @@
         <v>7</v>
       </c>
       <c r="D19" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.7326732673267328E-2</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F19" s="35" t="s">
+        <v>214</v>
+      </c>
+      <c r="G19" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>7 (1,7%)</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="35" t="s">
         <v>217</v>
       </c>
@@ -1585,17 +1711,28 @@
         <v>31</v>
       </c>
       <c r="D20" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.6732673267326731E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F20" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="G20" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>31 (7,7%)</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="38" t="s">
         <v>227</v>
       </c>
       <c r="D21" s="37"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F21" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="G21" s="35"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="35" t="s">
         <v>228</v>
       </c>
@@ -1603,11 +1740,18 @@
         <v>20</v>
       </c>
       <c r="D22" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.9504950495049507E-2</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F22" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="G22" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>20 (5%)</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="35" t="s">
         <v>229</v>
       </c>
@@ -1615,11 +1759,18 @@
         <v>365</v>
       </c>
       <c r="D23" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.90346534653465349</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F23" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="G23" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>365 (90,3%)</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="35" t="s">
         <v>217</v>
       </c>
@@ -1627,17 +1778,28 @@
         <v>19</v>
       </c>
       <c r="D24" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.702970297029703E-2</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F24" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="G24" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>19 (4,7%)</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="38" t="s">
         <v>230</v>
       </c>
       <c r="D25" s="37"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F25" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="G25" s="35"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="35" t="s">
         <v>233</v>
       </c>
@@ -1645,11 +1807,18 @@
         <v>212</v>
       </c>
       <c r="D26" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.52475247524752477</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F26" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="G26" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>212 (52,5%)</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="35" t="s">
         <v>232</v>
       </c>
@@ -1657,11 +1826,18 @@
         <v>161</v>
       </c>
       <c r="D27" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.39851485148514854</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F27" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="G27" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>161 (39,9%)</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="35" t="s">
         <v>234</v>
       </c>
@@ -1669,11 +1845,18 @@
         <v>19</v>
       </c>
       <c r="D28" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.702970297029703E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F28" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="G28" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>19 (4,7%)</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="35" t="s">
         <v>217</v>
       </c>
@@ -1681,11 +1864,18 @@
         <v>10</v>
       </c>
       <c r="D29" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.4752475247524754E-2</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F29" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="G29" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>10 (2,5%)</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="35" t="s">
         <v>231</v>
       </c>
@@ -1693,17 +1883,28 @@
         <v>2</v>
       </c>
       <c r="D30" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.9504950495049506E-3</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F30" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="G30" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>2 (0,5%)</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="38" t="s">
         <v>235</v>
       </c>
       <c r="D31" s="37"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F31" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="G31" s="35"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" s="35" t="s">
         <v>236</v>
       </c>
@@ -1711,11 +1912,18 @@
         <v>257</v>
       </c>
       <c r="D32" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.63613861386138615</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F32" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="G32" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>257 (63,6%)</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="35" t="s">
         <v>237</v>
       </c>
@@ -1723,11 +1931,18 @@
         <v>146</v>
       </c>
       <c r="D33" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.36138613861386137</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F33" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="G33" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>146 (36,1%)</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="35" t="s">
         <v>217</v>
       </c>
@@ -1735,8 +1950,15 @@
         <v>1</v>
       </c>
       <c r="D34" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.4752475247524753E-3</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="G34" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>1 (0,2%)</v>
       </c>
     </row>
   </sheetData>
@@ -1749,7 +1971,7 @@
   <dimension ref="B1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1764,14 +1986,14 @@
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="41" t="s">
         <v>238</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39" t="s">
+      <c r="D2" s="41"/>
+      <c r="E2" s="41" t="s">
         <v>239</v>
       </c>
-      <c r="F2" s="39"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="34" t="s">
@@ -2061,7 +2283,7 @@
       <c r="B24" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="39" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2077,7 +2299,7 @@
         <f>E5 &amp; " (" &amp; ROUND(100*F5,1) &amp; "%)"</f>
         <v>85 (32,3%)</v>
       </c>
-      <c r="E25" s="40"/>
+      <c r="E25" s="39"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="35" t="s">
@@ -2091,13 +2313,13 @@
         <f>E6 &amp; " (" &amp; ROUND(100*F6,1) &amp; "%)"</f>
         <v>16 (16,8%)</v>
       </c>
-      <c r="E26" s="40"/>
+      <c r="E26" s="39"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="40" t="s">
+      <c r="E27" s="39" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2110,10 +2332,10 @@
         <v>24 (70,6%)</v>
       </c>
       <c r="D28" s="36" t="str">
-        <f>E8 &amp; " (" &amp; ROUND(100*F8,1) &amp; "%)"</f>
+        <f t="shared" ref="D28:D33" si="3">E8 &amp; " (" &amp; ROUND(100*F8,1) &amp; "%)"</f>
         <v>10 (29,4%)</v>
       </c>
-      <c r="E28" s="40"/>
+      <c r="E28" s="39"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" s="35" t="s">
@@ -2124,10 +2346,10 @@
         <v>27 (67,5%)</v>
       </c>
       <c r="D29" s="36" t="str">
-        <f>E9 &amp; " (" &amp; ROUND(100*F9,1) &amp; "%)"</f>
+        <f t="shared" si="3"/>
         <v>13 (32,5%)</v>
       </c>
-      <c r="E29" s="40"/>
+      <c r="E29" s="39"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" s="35" t="s">
@@ -2138,10 +2360,10 @@
         <v>68 (64,2%)</v>
       </c>
       <c r="D30" s="36" t="str">
-        <f>E10 &amp; " (" &amp; ROUND(100*F10,1) &amp; "%)"</f>
+        <f t="shared" si="3"/>
         <v>38 (35,8%)</v>
       </c>
-      <c r="E30" s="40"/>
+      <c r="E30" s="39"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" s="35" t="s">
@@ -2152,10 +2374,10 @@
         <v>89 (70,6%)</v>
       </c>
       <c r="D31" s="36" t="str">
-        <f>E11 &amp; " (" &amp; ROUND(100*F11,1) &amp; "%)"</f>
+        <f t="shared" si="3"/>
         <v>37 (29,4%)</v>
       </c>
-      <c r="E31" s="40"/>
+      <c r="E31" s="39"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" s="35" t="s">
@@ -2166,10 +2388,10 @@
         <v>42 (54,5%)</v>
       </c>
       <c r="D32" s="36" t="str">
-        <f>E12 &amp; " (" &amp; ROUND(100*F12,1) &amp; "%)"</f>
+        <f t="shared" si="3"/>
         <v>35 (45,5%)</v>
       </c>
-      <c r="E32" s="40"/>
+      <c r="E32" s="39"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="35" t="s">
@@ -2180,16 +2402,16 @@
         <v>5 (31,3%)</v>
       </c>
       <c r="D33" s="36" t="str">
-        <f>E13 &amp; " (" &amp; ROUND(100*F13,1) &amp; "%)"</f>
+        <f t="shared" si="3"/>
         <v>11 (68,8%)</v>
       </c>
-      <c r="E33" s="40"/>
+      <c r="E33" s="39"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="E34" s="40" t="s">
+      <c r="E34" s="39" t="s">
         <v>244</v>
       </c>
     </row>
@@ -2205,7 +2427,7 @@
         <f>E15 &amp; " (" &amp; ROUND(100*F15,1) &amp; "%)"</f>
         <v>50 (26,6%)</v>
       </c>
-      <c r="E35" s="40"/>
+      <c r="E35" s="39"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="35" t="s">
@@ -2219,7 +2441,7 @@
         <f>E16 &amp; " (" &amp; ROUND(100*F16,1) &amp; "%)"</f>
         <v>31 (32,6%)</v>
       </c>
-      <c r="E36" s="40"/>
+      <c r="E36" s="39"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="35" t="s">
@@ -2233,7 +2455,7 @@
         <f>E17 &amp; " (" &amp; ROUND(100*F17,1) &amp; "%)"</f>
         <v>43 (52,4%)</v>
       </c>
-      <c r="E37" s="40"/>
+      <c r="E37" s="39"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="35" t="s">
@@ -2247,7 +2469,7 @@
         <f>E18 &amp; " (" &amp; ROUND(100*F18,1) &amp; "%)"</f>
         <v>4 (57,1%)</v>
       </c>
-      <c r="E38" s="40"/>
+      <c r="E38" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>